<commit_message>
edit data sample type from C to cast
</commit_message>
<xml_diff>
--- a/data/input/DOC_20240209_EN712_wNPOCandTNdata.2024.04.22_edited.xlsx
+++ b/data/input/DOC_20240209_EN712_wNPOCandTNdata.2024.04.22_edited.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19476" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10452"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>L4</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Notes during lab analysis</t>
+  </si>
+  <si>
+    <t>cast</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9F5FCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -796,7 +831,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T23" sqref="T23"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,63 +850,63 @@
   <sheetData>
     <row r="1" spans="1:20" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="P1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>20240209</v>
@@ -886,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -898,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="16">
@@ -911,7 +946,7 @@
         <v>45403</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="14">
         <v>86.006566181536598</v>
@@ -926,7 +961,7 @@
     </row>
     <row r="3" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="7">
         <v>20240210</v>
@@ -938,10 +973,10 @@
         <v>77</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G3" s="7">
         <v>2</v>
@@ -953,7 +988,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="16">
@@ -966,7 +1001,7 @@
         <v>45403</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="14">
         <v>68.167017378181697</v>
@@ -981,7 +1016,7 @@
     </row>
     <row r="4" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7">
         <v>20240210</v>
@@ -993,10 +1028,10 @@
         <v>77</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G4" s="7">
         <v>2</v>
@@ -1008,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="16">
@@ -1021,7 +1056,7 @@
         <v>45403</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="14">
         <v>67.797405865741098</v>
@@ -1036,7 +1071,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>20240210</v>
@@ -1048,10 +1083,10 @@
         <v>94</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G5" s="4">
         <v>5</v>
@@ -1063,7 +1098,7 @@
         <v>89</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="16">
@@ -1076,7 +1111,7 @@
         <v>45403</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="14">
         <v>64.292922832677505</v>
@@ -1091,7 +1126,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4">
         <v>20240210</v>
@@ -1103,10 +1138,10 @@
         <v>94</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G6" s="4">
         <v>5</v>
@@ -1118,7 +1153,7 @@
         <v>33</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="16">
@@ -1131,7 +1166,7 @@
         <v>45403</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="14">
         <v>65.111786649858303</v>
@@ -1146,7 +1181,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4">
         <v>20240210</v>
@@ -1158,10 +1193,10 @@
         <v>94</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G7" s="4">
         <v>5</v>
@@ -1173,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="16">
@@ -1186,7 +1221,7 @@
         <v>45403</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="14">
         <v>63.253619063991202</v>
@@ -1201,7 +1236,7 @@
     </row>
     <row r="8" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7">
         <v>20240210</v>
@@ -1213,10 +1248,10 @@
         <v>124</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G8" s="7">
         <v>6</v>
@@ -1228,7 +1263,7 @@
         <v>102</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="16">
@@ -1241,7 +1276,7 @@
         <v>45403</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q8" s="14">
         <v>60.359943774922598</v>
@@ -1256,7 +1291,7 @@
     </row>
     <row r="9" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7">
         <v>20240210</v>
@@ -1268,10 +1303,10 @@
         <v>124</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G9" s="7">
         <v>6</v>
@@ -1283,7 +1318,7 @@
         <v>56</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="16">
@@ -1296,7 +1331,7 @@
         <v>45403</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q9" s="14">
         <v>64.909831580234595</v>
@@ -1311,7 +1346,7 @@
     </row>
     <row r="10" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7">
         <v>20240210</v>
@@ -1323,10 +1358,10 @@
         <v>124</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G10" s="7">
         <v>6</v>
@@ -1338,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="16">
@@ -1351,7 +1386,7 @@
         <v>45403</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="14">
         <v>68.332021220546594</v>
@@ -1366,7 +1401,7 @@
     </row>
     <row r="11" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7">
         <v>20240210</v>
@@ -1378,10 +1413,10 @@
         <v>124</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G11" s="7">
         <v>6</v>
@@ -1393,10 +1428,10 @@
         <v>3</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L11" s="16">
         <v>1</v>
@@ -1408,7 +1443,7 @@
         <v>45403</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q11" s="14">
         <v>65.095329616684197</v>
@@ -1423,7 +1458,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4">
         <v>20240211</v>
@@ -1435,10 +1470,10 @@
         <v>447</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G12" s="4">
         <v>7</v>
@@ -1450,7 +1485,7 @@
         <v>440</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="16">
@@ -1463,7 +1498,7 @@
         <v>45403</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q12" s="14">
         <v>46.736696040019197</v>
@@ -1478,7 +1513,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4">
         <v>20240211</v>
@@ -1490,10 +1525,10 @@
         <v>447</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4">
         <v>7</v>
@@ -1505,7 +1540,7 @@
         <v>130</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="16">
@@ -1518,7 +1553,7 @@
         <v>45403</v>
       </c>
       <c r="P13" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q13" s="14">
         <v>56.025845967346399</v>
@@ -1533,7 +1568,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="4">
         <v>20240211</v>
@@ -1545,10 +1580,10 @@
         <v>447</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G14" s="4">
         <v>7</v>
@@ -1560,7 +1595,7 @@
         <v>15</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="16">
@@ -1573,7 +1608,7 @@
         <v>45403</v>
       </c>
       <c r="P14" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="14">
         <v>64.851059544692106</v>
@@ -1588,7 +1623,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4">
         <v>20240211</v>
@@ -1600,10 +1635,10 @@
         <v>447</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4">
         <v>7</v>
@@ -1615,7 +1650,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="16">
@@ -1628,7 +1663,7 @@
         <v>45403</v>
       </c>
       <c r="P15" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q15" s="14">
         <v>63.755216279447502</v>
@@ -1643,7 +1678,7 @@
     </row>
     <row r="16" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="7">
         <v>20240211</v>
@@ -1655,10 +1690,10 @@
         <v>1591</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G16" s="7">
         <v>10</v>
@@ -1670,7 +1705,7 @@
         <v>500</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="16">
@@ -1683,7 +1718,7 @@
         <v>45403</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="14">
         <v>42.407023961922498</v>
@@ -1698,7 +1733,7 @@
     </row>
     <row r="17" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="7">
         <v>20240211</v>
@@ -1710,10 +1745,10 @@
         <v>1591</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G17" s="7">
         <v>10</v>
@@ -1725,10 +1760,10 @@
         <v>500</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L17" s="16">
         <v>1</v>
@@ -1740,7 +1775,7 @@
         <v>45403</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q17" s="14">
         <v>47.056509303192499</v>
@@ -1755,7 +1790,7 @@
     </row>
     <row r="18" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="7">
         <v>20240211</v>
@@ -1767,10 +1802,10 @@
         <v>1591</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G18" s="7">
         <v>10</v>
@@ -1782,7 +1817,7 @@
         <v>120</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="16">
@@ -1795,7 +1830,7 @@
         <v>45403</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q18" s="14">
         <v>55.233589934643597</v>
@@ -1810,7 +1845,7 @@
     </row>
     <row r="19" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="7">
         <v>20240211</v>
@@ -1822,10 +1857,10 @@
         <v>1591</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G19" s="7">
         <v>10</v>
@@ -1837,7 +1872,7 @@
         <v>26</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="16">
@@ -1850,7 +1885,7 @@
         <v>45403</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q19" s="14">
         <v>60.782209549388497</v>
@@ -1865,7 +1900,7 @@
     </row>
     <row r="20" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="7">
         <v>20240211</v>
@@ -1877,10 +1912,10 @@
         <v>1591</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G20" s="7">
         <v>10</v>
@@ -1892,7 +1927,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="16">
@@ -1905,7 +1940,7 @@
         <v>45403</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q20" s="14">
         <v>63.565751027146597</v>
@@ -1920,7 +1955,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="4">
         <v>20240211</v>
@@ -1932,10 +1967,10 @@
         <v>210</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G21" s="4">
         <v>11</v>
@@ -1947,7 +1982,7 @@
         <v>206</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="16">
@@ -1960,7 +1995,7 @@
         <v>45403</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q21" s="14">
         <v>45.182158768914903</v>
@@ -1975,7 +2010,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4">
         <v>20240211</v>
@@ -1987,10 +2022,10 @@
         <v>210</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G22" s="4">
         <v>11</v>
@@ -2002,7 +2037,7 @@
         <v>75</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="16">
@@ -2015,7 +2050,7 @@
         <v>45403</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q22" s="14">
         <v>55.578723267193098</v>
@@ -2030,7 +2065,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="4">
         <v>20240211</v>
@@ -2042,10 +2077,10 @@
         <v>210</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G23" s="4">
         <v>11</v>
@@ -2057,7 +2092,7 @@
         <v>3</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="16">
@@ -2070,7 +2105,7 @@
         <v>45403</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q23" s="14">
         <v>64.3714331675598</v>
@@ -2085,7 +2120,7 @@
     </row>
     <row r="24" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="7">
         <v>20240212</v>
@@ -2097,10 +2132,10 @@
         <v>140</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G24" s="7">
         <v>12</v>
@@ -2112,7 +2147,7 @@
         <v>135</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="16">
@@ -2125,7 +2160,7 @@
         <v>45403</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q24" s="14">
         <v>58.053821141727902</v>
@@ -2140,7 +2175,7 @@
     </row>
     <row r="25" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="7">
         <v>20240212</v>
@@ -2152,10 +2187,10 @@
         <v>140</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G25" s="7">
         <v>12</v>
@@ -2167,7 +2202,7 @@
         <v>36</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="16">
@@ -2180,7 +2215,7 @@
         <v>45403</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q25" s="14">
         <v>65.9013374575771</v>
@@ -2195,7 +2230,7 @@
     </row>
     <row r="26" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7">
         <v>20240212</v>
@@ -2207,10 +2242,10 @@
         <v>140</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G26" s="7">
         <v>12</v>
@@ -2222,7 +2257,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="16">
@@ -2235,7 +2270,7 @@
         <v>45403</v>
       </c>
       <c r="P26" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q26" s="14">
         <v>62.0968909285723</v>
@@ -2250,7 +2285,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4">
         <v>20240212</v>
@@ -2262,10 +2297,10 @@
         <v>65</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G27" s="4">
         <v>15</v>
@@ -2277,7 +2312,7 @@
         <v>40</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="16">
@@ -2290,7 +2325,7 @@
         <v>45403</v>
       </c>
       <c r="P27" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q27" s="14">
         <v>68.014685224334997</v>
@@ -2305,7 +2340,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4">
         <v>20240212</v>
@@ -2317,10 +2352,10 @@
         <v>65</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G28" s="4">
         <v>15</v>
@@ -2332,7 +2367,7 @@
         <v>3</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="16">
@@ -2345,7 +2380,7 @@
         <v>45403</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q28" s="14">
         <v>64.1186985403656</v>
@@ -2360,7 +2395,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="4">
         <v>20240212</v>
@@ -2372,10 +2407,10 @@
         <v>65</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G29" s="4">
         <v>15</v>
@@ -2387,10 +2422,10 @@
         <v>3</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L29" s="16">
         <v>1</v>
@@ -2402,7 +2437,7 @@
         <v>45403</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q29" s="14">
         <v>69.239674949792402</v>
@@ -2417,7 +2452,7 @@
     </row>
     <row r="30" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="7">
         <v>20240213</v>
@@ -2429,10 +2464,10 @@
         <v>55</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G30" s="7">
         <v>16</v>
@@ -2444,7 +2479,7 @@
         <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K30" s="9"/>
       <c r="L30" s="16">
@@ -2457,7 +2492,7 @@
         <v>45403</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q30" s="14">
         <v>68.123015552322798</v>
@@ -2472,7 +2507,7 @@
     </row>
     <row r="31" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="7">
         <v>20240213</v>
@@ -2484,10 +2519,10 @@
         <v>55</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G31" s="7">
         <v>16</v>
@@ -2499,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="16">
@@ -2512,7 +2547,7 @@
         <v>45403</v>
       </c>
       <c r="P31" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q31" s="14">
         <v>68.486547602311902</v>
@@ -2527,7 +2562,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="4">
         <v>20240213</v>
@@ -2539,10 +2574,10 @@
         <v>46</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G32" s="4">
         <v>17</v>
@@ -2554,7 +2589,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="16">
@@ -2567,7 +2602,7 @@
         <v>45403</v>
       </c>
       <c r="P32" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q32" s="14">
         <v>74.369407798694397</v>
@@ -2582,7 +2617,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="4">
         <v>20240213</v>
@@ -2594,10 +2629,10 @@
         <v>46</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="G33" s="4">
         <v>17</v>
@@ -2609,10 +2644,10 @@
         <v>3</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L33" s="16">
         <v>1</v>
@@ -2624,7 +2659,7 @@
         <v>45403</v>
       </c>
       <c r="P33" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q33" s="14">
         <v>71.196601915864605</v>
@@ -2639,7 +2674,7 @@
     </row>
     <row r="34" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="7">
         <v>20240213</v>
@@ -2651,10 +2686,10 @@
         <v>20</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="G34" s="7">
         <v>20</v>
@@ -2666,7 +2701,7 @@
         <v>3</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K34" s="9"/>
       <c r="L34" s="16">
@@ -2679,7 +2714,7 @@
         <v>45403</v>
       </c>
       <c r="P34" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q34" s="14">
         <v>77.192142585006494</v>
@@ -2694,23 +2729,23 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L35" s="16">
         <v>1</v>
@@ -2722,7 +2757,7 @@
         <v>45403</v>
       </c>
       <c r="P35" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q35" s="14">
         <v>6.7150288268084903</v>
@@ -2737,23 +2772,23 @@
     </row>
     <row r="36" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
       <c r="J36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L36" s="16">
         <v>1</v>
@@ -2765,7 +2800,7 @@
         <v>45403</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q36" s="14">
         <v>4.9218437535887603</v>
@@ -2793,57 +2828,74 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:I2 A3:A36">
-    <cfRule type="beginsWith" dxfId="15" priority="40" operator="beginsWith" text="r">
+    <cfRule type="beginsWith" dxfId="20" priority="45" operator="beginsWith" text="r">
       <formula>LEFT(A2,LEN("r"))="r"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="41" operator="beginsWith" text="f">
+    <cfRule type="beginsWith" dxfId="19" priority="46" operator="beginsWith" text="f">
       <formula>LEFT(A2,LEN("f"))="f"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="42" operator="beginsWith" text="n">
+    <cfRule type="beginsWith" dxfId="18" priority="47" operator="beginsWith" text="n">
       <formula>LEFT(A2,LEN("n"))="n"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="43" operator="beginsWith" text="y">
+    <cfRule type="beginsWith" dxfId="17" priority="48" operator="beginsWith" text="y">
       <formula>LEFT(A2,LEN("y"))="y"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="11" priority="44">
+    <cfRule type="containsBlanks" dxfId="16" priority="49">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:I34 F35:F36">
-    <cfRule type="beginsWith" dxfId="10" priority="7" operator="beginsWith" text="r">
+  <conditionalFormatting sqref="B3:E34 F35:F36 G3:I34">
+    <cfRule type="beginsWith" dxfId="15" priority="12" operator="beginsWith" text="r">
       <formula>LEFT(B3,LEN("r"))="r"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="8" operator="beginsWith" text="f">
+    <cfRule type="beginsWith" dxfId="14" priority="13" operator="beginsWith" text="f">
       <formula>LEFT(B3,LEN("f"))="f"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="9" operator="beginsWith" text="n">
+    <cfRule type="beginsWith" dxfId="13" priority="14" operator="beginsWith" text="n">
       <formula>LEFT(B3,LEN("n"))="n"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="10" operator="beginsWith" text="y">
+    <cfRule type="beginsWith" dxfId="12" priority="15" operator="beginsWith" text="y">
       <formula>LEFT(B3,LEN("y"))="y"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="6" priority="11">
+    <cfRule type="containsBlanks" dxfId="11" priority="16">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J36">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="11">
       <formula>LEN(TRIM(J2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F34">
+    <cfRule type="beginsWith" dxfId="4" priority="1" operator="beginsWith" text="r">
+      <formula>LEFT(F3,LEN("r"))="r"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="f">
+      <formula>LEFT(F3,LEN("f"))="f"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" operator="beginsWith" text="n">
+      <formula>LEFT(F3,LEN("n"))="n"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="4" operator="beginsWith" text="y">
+      <formula>LEFT(F3,LEN("y"))="y"</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2852,14 +2904,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e362b6aa-9e52-454d-a744-a011f894490f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087D5BADFAE2D5F4C918B95ED792D7747" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5e31e831f5d10d6e2842525e156c885">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e362b6aa-9e52-454d-a744-a011f894490f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="033d181dc29646ef2c939bb4990c3b97" ns3:_="">
     <xsd:import namespace="e362b6aa-9e52-454d-a744-a011f894490f"/>
@@ -3041,6 +3085,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e362b6aa-9e52-454d-a744-a011f894490f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3051,22 +3103,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBAD766-690B-4B4D-8BA3-45BBCD0E4195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e362b6aa-9e52-454d-a744-a011f894490f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6760C1B4-AA74-49DA-BD0D-5CB8CAEA2C03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3084,6 +3120,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EBAD766-690B-4B4D-8BA3-45BBCD0E4195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e362b6aa-9e52-454d-a744-a011f894490f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C56E6CDE-B1D8-4B8C-A235-CFA6F399302F}">
   <ds:schemaRefs>

</xml_diff>